<commit_message>
Update per 21st of june.
</commit_message>
<xml_diff>
--- a/Part1b_Dataset preparation_Convert_to_specific_datatypes_ranking_table.xlsx
+++ b/Part1b_Dataset preparation_Convert_to_specific_datatypes_ranking_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Human use" sheetId="3" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="91">
-  <si>
-    <t>fme_feature_type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="78">
   <si>
     <t>Lagoon fishing or aquaculture</t>
   </si>
@@ -299,21 +296,6 @@
     <t>Historical monu- ments</t>
   </si>
   <si>
-    <t>Coast_Class</t>
-  </si>
-  <si>
-    <t>CoastClass</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>AttributeFilter1</t>
   </si>
   <si>
@@ -332,15 +314,9 @@
     <t>NewAttributeValue</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>Hotels with rooms &gt; 10</t>
   </si>
   <si>
-    <t>Rankings_Coast_Class</t>
-  </si>
-  <si>
     <t>Canoes</t>
   </si>
   <si>
@@ -348,21 +324,6 @@
   </si>
   <si>
     <t>&gt;50</t>
-  </si>
-  <si>
-    <t>Turtles</t>
-  </si>
-  <si>
-    <t>Nests</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Tutles</t>
-  </si>
-  <si>
-    <t>Number</t>
   </si>
   <si>
     <t>Mangroves</t>
@@ -940,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C10:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:P31"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,495 +922,495 @@
   <sheetData>
     <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>26</v>
-      </c>
       <c r="E10" s="9" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C11" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L11" t="str">
-        <f>D11</f>
+        <f t="shared" ref="L11:L23" si="0">D11</f>
         <v>Fishing Village with canoes&lt; 50</v>
       </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="L12" t="str">
-        <f>D12</f>
+        <f t="shared" si="0"/>
         <v>Fishing Village with canoes &gt;50</v>
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C13" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
       <c r="L13" t="str">
-        <f>D13</f>
+        <f t="shared" si="0"/>
         <v>Fishing Village with beach seine net&gt; 5</v>
       </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C14" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
       <c r="L14" t="str">
-        <f>D14</f>
+        <f t="shared" si="0"/>
         <v>Fishing Village with beach seine net&lt; 5</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="L15" t="str">
-        <f>D15</f>
+        <f t="shared" si="0"/>
         <v>Lagoon fishing or aquaculture</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
       <c r="L16" t="str">
-        <f>D16</f>
+        <f t="shared" si="0"/>
         <v>Salt production</v>
       </c>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
       <c r="L17" t="str">
-        <f>D17</f>
+        <f t="shared" si="0"/>
         <v>Major ports</v>
       </c>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
       <c r="L18" t="str">
-        <f>D18</f>
+        <f t="shared" si="0"/>
         <v>Marine water intakes</v>
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
       <c r="J19" s="16"/>
       <c r="L19" t="str">
-        <f>D19</f>
+        <f t="shared" si="0"/>
         <v>Coastal farming</v>
       </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
       <c r="L20" t="str">
-        <f>D20</f>
+        <f t="shared" si="0"/>
         <v>Hotels with rooms &gt; 10</v>
       </c>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
       <c r="L21" t="str">
-        <f>D21</f>
+        <f t="shared" si="0"/>
         <v>Hotels with rooms &lt; 20</v>
       </c>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
       <c r="L22" t="str">
-        <f>D22</f>
+        <f t="shared" si="0"/>
         <v>Beach for recreational purposes</v>
       </c>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
       <c r="L23" t="str">
-        <f>D23</f>
+        <f t="shared" si="0"/>
         <v>Historical monu- ments</v>
       </c>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C28" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="J28" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="K28" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="L28" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H28" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="15" t="s">
+      <c r="M28" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="N28" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="K28" s="15" t="s">
+      <c r="O28" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="L28" s="15" t="s">
+      <c r="P28" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="M28" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N28" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O28" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P28" s="15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="29" spans="3:16" ht="76.5" x14ac:dyDescent="0.25">
       <c r="C29" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="K29" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="L29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="M29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N29" s="2" t="s">
+      <c r="O29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="P29" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="P29" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" s="9" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D30" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="G30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30" s="11" t="s">
+      <c r="N30" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="N30" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="O30" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P30" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E31" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="G31" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="H31" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="I31" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="J31" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="K31" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="L31" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="M31" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="N31" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="O31" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="P31" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1461,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:Q31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,588 +1444,517 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>26</v>
-      </c>
       <c r="E10" s="9" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N10" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="O10" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="P10" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q10" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="R10" s="9" t="s">
-        <v>47</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="N11" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="O11" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>48</v>
-      </c>
-      <c r="R11" t="str">
-        <f>D11</f>
-        <v>Sandy Beach Fine grained, low slope</v>
-      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="18"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
-      <c r="Q12" t="s">
-        <v>48</v>
-      </c>
-      <c r="R12" t="str">
-        <f>D12</f>
-        <v>Sandy Beach Coarse and mobile</v>
-      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="P13" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>48</v>
-      </c>
-      <c r="R13" t="str">
-        <f>D13</f>
-        <v>Sandy Beach Turtle nesting sites</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
-      </c>
-      <c r="N14" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="O14" s="16" t="s">
-        <v>58</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
       <c r="P14" s="16"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
       <c r="P15" s="16"/>
-      <c r="Q15" t="s">
-        <v>48</v>
-      </c>
-      <c r="R15" t="str">
-        <f>D15</f>
-        <v>Rock Steep Exposed</v>
-      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" t="s">
-        <v>68</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="N16" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="O16" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="P16" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>48</v>
-      </c>
-      <c r="R16" t="str">
-        <f>D16</f>
-        <v>Rock Moderate Slope exposed</v>
-      </c>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
       <c r="P17" s="16"/>
-      <c r="Q17" t="s">
-        <v>48</v>
-      </c>
-      <c r="R17" t="str">
-        <f>D17</f>
-        <v>Mixed Rock and Sandy Beach</v>
-      </c>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
       <c r="P18" s="16"/>
-      <c r="Q18" t="s">
-        <v>48</v>
-      </c>
-      <c r="R18" t="str">
-        <f>D18</f>
-        <v>Rocky Flats with crevices</v>
-      </c>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="G19" s="20"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
       <c r="P19" s="16"/>
-      <c r="Q19" t="s">
-        <v>48</v>
-      </c>
-      <c r="R19" t="str">
-        <f>D19</f>
-        <v>Intertidal Rocks with algae</v>
-      </c>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F20" t="s">
-        <v>72</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="N20" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="O20" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="P20" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>48</v>
-      </c>
-      <c r="R20" t="str">
-        <f>D20</f>
-        <v>Open Coastal Lagoon</v>
-      </c>
-    </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C21" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="F21" t="s">
-        <v>73</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
       <c r="P21" s="16"/>
-      <c r="R21" t="str">
-        <f>D21</f>
-        <v>Semi Closed Lagoon</v>
-      </c>
-    </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
       <c r="N22" s="16"/>
       <c r="O22" s="16"/>
       <c r="P22" s="16"/>
-      <c r="R22" t="str">
-        <f>D22</f>
-        <v>Open Coastal Lagoon important for birds</v>
-      </c>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C23" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>75</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
       <c r="P23" s="16"/>
-      <c r="R23" t="str">
-        <f>D23</f>
-        <v>Semi-closed Lagoons important for birds</v>
-      </c>
-    </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C24" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F24" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
       <c r="P24" s="16"/>
-      <c r="R24" t="str">
-        <f>D24</f>
-        <v>Mangroves</v>
-      </c>
-    </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D25" s="19"/>
-      <c r="L25">
-        <f>D25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q28" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" ht="72.75" x14ac:dyDescent="0.25">
+      <c r="C29" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28" s="8" t="s">
+      <c r="D29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C30" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N28" s="8" t="s">
+      <c r="E30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="O28" s="8" t="s">
+      <c r="F30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q28" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="3:18" ht="72.75" x14ac:dyDescent="0.25">
-      <c r="C29" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q29" s="3" t="s">
+      <c r="I30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" t="s">
+        <v>56</v>
+      </c>
+      <c r="K31" t="s">
+        <v>57</v>
+      </c>
+      <c r="L31" t="s">
+        <v>58</v>
+      </c>
+      <c r="M31" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C30" s="9" t="s">
+      <c r="N31" t="s">
+        <v>60</v>
+      </c>
+      <c r="O31" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="O30" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q30" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="P31" t="s">
         <v>62</v>
       </c>
-      <c r="D31" t="s">
+      <c r="Q31" t="s">
         <v>63</v>
-      </c>
-      <c r="E31" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" t="s">
-        <v>65</v>
-      </c>
-      <c r="G31" t="s">
-        <v>66</v>
-      </c>
-      <c r="H31" t="s">
-        <v>67</v>
-      </c>
-      <c r="I31" t="s">
-        <v>68</v>
-      </c>
-      <c r="J31" t="s">
-        <v>69</v>
-      </c>
-      <c r="K31" t="s">
-        <v>70</v>
-      </c>
-      <c r="L31" t="s">
-        <v>71</v>
-      </c>
-      <c r="M31" t="s">
-        <v>72</v>
-      </c>
-      <c r="N31" t="s">
-        <v>73</v>
-      </c>
-      <c r="O31" t="s">
-        <v>74</v>
-      </c>
-      <c r="P31" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>